<commit_message>
Grouping Variables For Easier Processing
Updates:
- Grouped each variable in meta excel;
- Uploaded Load&Clean Python script.
</commit_message>
<xml_diff>
--- a/column_meta.xlsx
+++ b/column_meta.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$84</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="197">
   <si>
     <t>HasDetections</t>
   </si>
@@ -160,12 +160,6 @@
     <t xml:space="preserve">SkuEdition </t>
   </si>
   <si>
-    <t xml:space="preserve"> The goal of this feature is to use the Product Type defined in the MSDN to map to a 'SKU</t>
-  </si>
-  <si>
-    <t>Edition' is a string value that is in one of three classes of results. The design must hand each class.</t>
-  </si>
-  <si>
     <t xml:space="preserve">IsProtected </t>
   </si>
   <si>
@@ -671,6 +665,10 @@
   </si>
   <si>
     <t>MetaData详细描述请参考这个网址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> The goal of this feature is to use the Product Type defined in the MSDN to map to a 'SKU Edition' is a string value that is in one of three classes of results. The design must hand each class.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1042,34 +1040,35 @@
   <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="7.90625" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" customWidth="1"/>
     <col min="6" max="6" width="52.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
         <v>137</v>
       </c>
-      <c r="B1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C1" t="s">
-        <v>139</v>
-      </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1080,10 +1079,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1094,7 +1096,14 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="str">
+        <f>"'"&amp;A3&amp;"':"&amp;D3&amp;","</f>
+        <v>'ProductName ':4,</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1105,7 +1114,14 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F67" si="0">"'"&amp;A4&amp;"':"&amp;D4&amp;","</f>
+        <v>'EngineVersion ':4,</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1116,7 +1132,14 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>'AppVersion ':4,</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1127,7 +1150,14 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>'AvSigVersion ':4,</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1138,7 +1168,14 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>'IsBeta ':1,</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1149,10 +1186,17 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>152</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>'RtpStateBitfield ':4,</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1163,10 +1207,17 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>149</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>150</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>'IsSxsPassiveMode ':1,</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1177,7 +1228,14 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>'DefaultBrowsersIdentifier ':4,</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1188,7 +1246,14 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>'AVProductStatesIdentifier ':4,</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,10 +1264,17 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>153</v>
+        <v>151</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>'AVProductsInstalled ':4,</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1213,10 +1285,17 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
       </c>
       <c r="E13">
         <v>1</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>'AVProductsEnabled ':4,</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1227,7 +1306,14 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>145</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>'HasTpm ':1,</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1238,7 +1324,14 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>'CountryIdentifier ':4,</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1249,10 +1342,17 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>'CityIdentifier ':4,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1260,10 +1360,17 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>'OrganizationIdentifier ':4,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1271,10 +1378,17 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>'GeoNameIdentifier ':4,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1282,21 +1396,35 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>'LocaleEnglishNameIdentifier ':4,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>'Platform ':4,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
@@ -1304,10 +1432,17 @@
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>'Processor ':4,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -1315,10 +1450,17 @@
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>'OsVer ':4,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
@@ -1326,10 +1468,17 @@
         <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>'OsBuild ':4,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -1337,13 +1486,20 @@
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>'OsSuite ':4,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -1351,719 +1507,1132 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>'OsPlatformSubRelease ':4,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>'OsBuildLab ':4,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B27" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>'SkuEdition ':4,</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" t="s">
         <v>145</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>'IsProtected ':1,</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B29" t="s">
         <v>49</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>161</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>'AutoSampleOptIn ':1,</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
         <v>162</v>
       </c>
-      <c r="C28" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" t="s">
-        <v>151</v>
-      </c>
-      <c r="E29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>'PuaMode ':1,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>53</v>
       </c>
-      <c r="C30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E30" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="C31" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>'SMode ':1,</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>'IeVerIdentifier ':4,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>'SmartScreen ':4,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>58</v>
       </c>
-      <c r="C33" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="C34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>'Firewall ':1,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>'UacLuaenable ':1,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B36" t="s">
         <v>61</v>
       </c>
-      <c r="B35" t="s">
-        <v>166</v>
-      </c>
-      <c r="C35" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="C36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_MDC2FormFactor ':3,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>63</v>
       </c>
-      <c r="C36" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="C37" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_DeviceFamily ':3,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B37" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OEMNameIdentifier ':3,</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>156</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OEMModelIdentifier ':3,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_ProcessorCoreCount ':3,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_ProcessorManufacturerIdentifier ':3,</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s">
         <v>14</v>
       </c>
       <c r="C42" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>167</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_ProcessorModelIdentifier ':2,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>192</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_ProcessorClass ':3,</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_PrimaryDiskTotalCapacity ':2,</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_PrimaryDiskTypeName ':3,</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" t="s">
         <v>168</v>
       </c>
-      <c r="E42" t="s">
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_SystemVolumeTotalCapacity ':2,</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_HasOpticalDiskDrive ':1,</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_TotalPhysicalRAM ':3,</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B43" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" t="s">
-        <v>140</v>
-      </c>
-      <c r="E43" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B46" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_ChassisTypeName ':3,</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>85</v>
       </c>
-      <c r="C49" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="C50" t="s">
+        <v>154</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_InternalPrimaryDiagonalDisplaySizeInInches ':2,</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>87</v>
       </c>
-      <c r="C50" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="C51" t="s">
+        <v>166</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_InternalPrimaryDisplayResolutionHorizontal ':2,</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>89</v>
       </c>
-      <c r="C51" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="C52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_InternalPrimaryDisplayResolutionVertical ':2,</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>91</v>
       </c>
-      <c r="C52" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="C53" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_PowerPlatformRoleName ':3,</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B53" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="B54" t="s">
         <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>172</v>
+        <v>170</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_InternalBatteryType ':3,</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B55" t="s">
         <v>14</v>
       </c>
       <c r="C55" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_InternalBatteryNumberOfCharges ':2,</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" t="s">
+        <v>172</v>
+      </c>
+      <c r="C56" t="s">
+        <v>166</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>193</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSVersion ':2,</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" t="s">
+        <v>143</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSArchitecture ':3,</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" t="s">
+        <v>173</v>
+      </c>
+      <c r="C58" t="s">
+        <v>143</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSBranch ':3,</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" t="s">
+        <v>143</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>141</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSBuildNumber ':3,</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" t="s">
+        <v>143</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>193</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSBuildRevision ':3,</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" t="s">
+        <v>138</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSEdition ':3,</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B56" t="s">
-        <v>174</v>
-      </c>
-      <c r="C56" t="s">
-        <v>168</v>
-      </c>
-      <c r="E56" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B57" t="s">
-        <v>176</v>
-      </c>
-      <c r="C57" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B58" t="s">
-        <v>175</v>
-      </c>
-      <c r="C58" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B59" t="s">
-        <v>177</v>
-      </c>
-      <c r="C59" t="s">
-        <v>145</v>
-      </c>
-      <c r="E59" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B60" t="s">
-        <v>178</v>
-      </c>
-      <c r="C60" t="s">
-        <v>145</v>
-      </c>
-      <c r="E60" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B61" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSSkuName ':3,</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>104</v>
       </c>
-      <c r="C62" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="C63" t="s">
+        <v>138</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSInstallTypeName ':3,</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B63" t="s">
-        <v>106</v>
-      </c>
-      <c r="C63" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="B64" t="s">
         <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
       </c>
       <c r="E64" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSInstallLanguageIdentifier ':3,</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B65" t="s">
         <v>14</v>
       </c>
       <c r="C65" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
       </c>
       <c r="E65" t="s">
+        <v>178</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSUILocaleIdentifier ':3,</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" t="s">
+        <v>179</v>
+      </c>
+      <c r="C66" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_OSWUAutoUpdateOptionsName ':3,</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="C67" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="0"/>
+        <v>'Census_IsPortableOperatingSystem ':1,</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B66" t="s">
-        <v>181</v>
-      </c>
-      <c r="C66" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="B68" t="s">
         <v>110</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C68" t="s">
+        <v>143</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" ref="F68:F84" si="1">"'"&amp;A68&amp;"':"&amp;D68&amp;","</f>
+        <v>'Census_GenuineStateName ':3,</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" t="s">
+        <v>112</v>
+      </c>
+      <c r="C69" t="s">
         <v>182</v>
       </c>
-      <c r="C67" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B68" t="s">
-        <v>112</v>
-      </c>
-      <c r="C68" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_ActivationChannel ':3,</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B69" t="s">
-        <v>114</v>
-      </c>
-      <c r="C69" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="B70" t="s">
         <v>14</v>
       </c>
       <c r="C70" t="s">
-        <v>151</v>
+        <v>149</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_IsFlightingInternal ':1,</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" t="s">
+        <v>115</v>
+      </c>
+      <c r="C71" t="s">
+        <v>149</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_IsFlightsDisabled ':1,</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>117</v>
       </c>
-      <c r="C71" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="C72" t="s">
+        <v>138</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_FlightRing ':3,</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B72" t="s">
-        <v>119</v>
-      </c>
-      <c r="C72" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="B73" t="s">
         <v>14</v>
       </c>
       <c r="C73" t="s">
-        <v>147</v>
+        <v>145</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_ThresholdOptIn ':1,</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B74" t="s">
         <v>14</v>
       </c>
       <c r="C74" t="s">
-        <v>156</v>
+        <v>154</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="F74" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_FirmwareManufacturerIdentifier ':2,</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B75" t="s">
         <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>196</v>
+        <v>194</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_FirmwareVersionIdentifier ':2,</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="F76" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_IsSecureBootEnabled ':1,</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B76" t="s">
-        <v>124</v>
-      </c>
-      <c r="C76" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="B77" t="s">
         <v>14</v>
       </c>
       <c r="C77" t="s">
-        <v>151</v>
+        <v>149</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="F77" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_IsWIMBootEnabled ':1,</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" t="s">
+        <v>145</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_IsVirtualDevice ':1,</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>127</v>
       </c>
-      <c r="C78" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="C79" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="F79" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_IsTouchEnabled ':1,</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>129</v>
       </c>
-      <c r="C79" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="C80" t="s">
+        <v>145</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_IsPenCapable ':1,</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>131</v>
       </c>
-      <c r="C80" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="C81" t="s">
+        <v>149</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="1"/>
+        <v>'Census_IsAlwaysOnAlwaysConnectedCapable ':1,</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>133</v>
       </c>
-      <c r="C81" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="C82" t="s">
+        <v>140</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="F82" t="str">
+        <f t="shared" si="1"/>
+        <v>'Wdft_IsGamer ':1,</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B82" t="s">
-        <v>135</v>
-      </c>
-      <c r="C82" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="B83" t="s">
         <v>14</v>
       </c>
       <c r="C83" t="s">
-        <v>190</v>
+        <v>188</v>
+      </c>
+      <c r="D83">
+        <v>4</v>
       </c>
       <c r="E83" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="F83" t="str">
+        <f t="shared" si="1"/>
+        <v>'Wdft_RegionIdentifier ':4,</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C84" t="s">
-        <v>147</v>
+        <v>145</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>